<commit_message>
Replacement of scripts creating db from scratch at particular moment correction of shift_no.sql adding new prcoderues and functions to handle topics from 1-5 tasks answer to 1-5 taks new backup of data base + db_fix for changes implemented 2023-01-16
</commit_message>
<xml_diff>
--- a/SQL/malfunction_task/Task split.xlsx
+++ b/SQL/malfunction_task/Task split.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\Repositories\Wsm_administrowanie\SQL\malfunction_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0082F190-38B8-40E2-8ACE-BA0925CA7287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF0DAB9-1CA9-450D-AC6D-4F5FDEFC3958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -438,45 +438,55 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Question 6 and 7 correction of procedures SumOfAllInactiveMinutes.sql for correct calculation Added answers for 6 and 7 question Added new procedure Unit_with_longest_malfunctions.sql and view statuses_fraction.sql
</commit_message>
<xml_diff>
--- a/SQL/malfunction_task/Task split.xlsx
+++ b/SQL/malfunction_task/Task split.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\Repositories\Wsm_administrowanie\SQL\malfunction_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF0DAB9-1CA9-450D-AC6D-4F5FDEFC3958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2096859-835D-4DCB-8F0A-CDC4EF00C5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -493,18 +493,22 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Question 9 and 10. removing firma, zlecenie status, estymata.sql modification of zlecenia.sql Task split.xlsx and Zadanie1  (1).docx
new fix, script, data and structure for element_typ, zlecenia, zlecenie-element, zlecenie_element_status, and two views v_elementy_do_realizacji_aggr.sql and v_nieskonczone_zlecenia.sql
</commit_message>
<xml_diff>
--- a/SQL/malfunction_task/Task split.xlsx
+++ b/SQL/malfunction_task/Task split.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\Repositories\Wsm_administrowanie\SQL\malfunction_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79467B5E-3F28-4D18-8E41-E73A5468D2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630F14F-27CE-4FEC-A88A-EC599FC94555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -526,18 +526,22 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Task 11 and 12 Update of data, change of strukture for usterka_status.sql, usterka_status, oddzial, added new script and new function
</commit_message>
<xml_diff>
--- a/SQL/malfunction_task/Task split.xlsx
+++ b/SQL/malfunction_task/Task split.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\Repositories\Wsm_administrowanie\SQL\malfunction_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630F14F-27CE-4FEC-A88A-EC599FC94555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C0221E-3339-4F82-8E87-D6EB38773F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -548,18 +548,22 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>